<commit_message>
Now shows bet type
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -11,6 +11,7 @@
     <sheet name="newSheet" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="newSheet1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="newSheet2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="newSheet3" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -913,4 +914,99 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>L3</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Now fills cell with colors
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -12,6 +12,17 @@
     <sheet name="newSheet1" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="newSheet2" sheetId="4" state="visible" r:id="rId4"/>
     <sheet name="newSheet3" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sheet5" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sheet6" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sheet7" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sheet8" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Sheet9" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet name="Sheet10" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet name="Sheet11" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet name="Sheet12" sheetId="14" state="visible" r:id="rId14"/>
+    <sheet name="Sheet13" sheetId="15" state="visible" r:id="rId15"/>
+    <sheet name="Sheet14" sheetId="16" state="visible" r:id="rId16"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -30,12 +41,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000FF"/>
+        <bgColor rgb="FF0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -50,9 +73,13 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -479,6 +506,1149 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-4</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-8</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B2" t="n">
+        <v>6</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B3" t="n">
+        <v>6</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B4" t="n">
+        <v>6</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B5" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B6" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B8" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B10" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B11" t="n">
+        <v>6</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B12" t="n">
+        <v>6</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B13" t="n">
+        <v>6</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B14" t="n">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B15" t="n">
+        <v>6</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B16" t="n">
+        <v>6</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B19" t="n">
+        <v>6</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B20" t="n">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B21" t="n">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B22" t="n">
+        <v>6</v>
+      </c>
+      <c r="C22" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>-35</v>
+      </c>
+      <c r="B23" t="n">
+        <v>6</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="C5" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
@@ -1009,4 +2179,806 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-4</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-8</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-12</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-16</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-24</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-28</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-32</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-36</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-40</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-44</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-48</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-52</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-56</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-60</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-64</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-68</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-72</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-76</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-80</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-84</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>-88</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>-3</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>ShoeTI</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PreTI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Board</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Bet Side</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Bet Amt</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Profits</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B2" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="E2" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C3" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B4" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C4" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B5" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C5" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B6" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C6" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B7" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C7" s="1" t="inlineStr">
+        <is>
+          <t>B</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B9" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>-6</v>
+      </c>
+      <c r="B10" t="n">
+        <v>-2</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>P</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>